<commit_message>
Test documentation for unit test course controller in backend added
</commit_message>
<xml_diff>
--- a/docs/test/Testconcept_OrganisationApp_MyCourses_Angel.xlsx
+++ b/docs/test/Testconcept_OrganisationApp_MyCourses_Angel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04_Coding\02_Projects\02_SE_Project_05\docs\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA48A30-BADE-4168-A5B3-C58007D57287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD6248-12DC-48DA-B767-223A39DFF62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38265" yWindow="3375" windowWidth="29070" windowHeight="15750" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="174">
   <si>
     <t>Leere Liste</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Test-Typ</t>
-  </si>
-  <si>
-    <t>Liste mit genau diesem Kurs</t>
   </si>
   <si>
     <t>Kurs nicht gelöscht</t>
@@ -472,13 +469,97 @@
   </si>
   <si>
     <t>integration_test/my_courses_page_integration_test.dart</t>
+  </si>
+  <si>
+    <t>organisation_app/controller/CourseController</t>
+  </si>
+  <si>
+    <t>ResponseStatusException Unauthorized</t>
+  </si>
+  <si>
+    <t>getCourseById</t>
+  </si>
+  <si>
+    <t>Es liegt Kursinformationen vor</t>
+  </si>
+  <si>
+    <t>Es liegen keine Kursinformationen vor</t>
+  </si>
+  <si>
+    <t>Kursinformationen</t>
+  </si>
+  <si>
+    <t>Gültige Kurs-Id</t>
+  </si>
+  <si>
+    <t>Ungültige Kurs-Id</t>
+  </si>
+  <si>
+    <t>ResponseStatusException NotFound</t>
+  </si>
+  <si>
+    <t>getAllTasksForCourse</t>
+  </si>
+  <si>
+    <t>Es liegen Tasks für den Kurs vor</t>
+  </si>
+  <si>
+    <t>Es liegen keine Tasks für den Kurs vor</t>
+  </si>
+  <si>
+    <t>Liste mit Tasks</t>
+  </si>
+  <si>
+    <t>createCourse</t>
+  </si>
+  <si>
+    <t>Kurs erfolgreich angelegt</t>
+  </si>
+  <si>
+    <t>Kurs nicht angelegt</t>
+  </si>
+  <si>
+    <t>Gültige Modul-Id und Username</t>
+  </si>
+  <si>
+    <t>Ungültige Modul-Id</t>
+  </si>
+  <si>
+    <t>Ungültiges Username</t>
+  </si>
+  <si>
+    <t>Erzeugter Kurs</t>
+  </si>
+  <si>
+    <t>ResponseStatusException Conflict</t>
+  </si>
+  <si>
+    <t>Es liegt genau eine Task für den Kurs vor</t>
+  </si>
+  <si>
+    <t>Kurs bereits vorhanden</t>
+  </si>
+  <si>
+    <t>updateCourseById</t>
+  </si>
+  <si>
+    <t>Gültige Kurs-Id und Kurs</t>
+  </si>
+  <si>
+    <t>Aktualisierter Kurs</t>
+  </si>
+  <si>
+    <t>Keine Ausgabe</t>
+  </si>
+  <si>
+    <t>Kein Kurs zu löschen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,8 +589,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,8 +622,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -653,13 +748,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -714,26 +836,850 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="96">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -754,6 +1700,142 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -1305,6 +2387,28 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1468,71 +2572,155 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A449AC-DC09-4BA4-B167-13CDD3BECA2A}" name="Table1" displayName="Table1" ref="A4:F15" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A449AC-DC09-4BA4-B167-13CDD3BECA2A}" name="Table1" displayName="Table1" ref="A4:F15" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93" totalsRowBorderDxfId="92">
   <autoFilter ref="A4:F15" xr:uid="{36A449AC-DC09-4BA4-B167-13CDD3BECA2A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{507A3FF2-9B07-462C-A22C-8B11345F819E}" name="Ort" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{07657F8A-5478-4DE7-8068-150C2CFA1187}" name="Typ" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{14093B07-E295-464C-BF31-4348B1CFF9BC}" name="Komponente-Datei" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{3D56AFAA-FFDA-43A3-BB43-5016E1E890FA}" name="Klasse" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{F84C3C09-490B-4651-81C6-6C8B08C187FF}" name="Methode" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{42935E76-B357-4DF0-A865-8B148F93BB65}" name="Test-Datei" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{507A3FF2-9B07-462C-A22C-8B11345F819E}" name="Ort" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{07657F8A-5478-4DE7-8068-150C2CFA1187}" name="Typ" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{14093B07-E295-464C-BF31-4348B1CFF9BC}" name="Komponente-Datei" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{3D56AFAA-FFDA-43A3-BB43-5016E1E890FA}" name="Klasse" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{F84C3C09-490B-4651-81C6-6C8B08C187FF}" name="Methode" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{42935E76-B357-4DF0-A865-8B148F93BB65}" name="Test-Datei" dataDxfId="86"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{DD8FE11C-2438-4049-A42D-CF49EF196CF3}" name="Table911" displayName="Table911" ref="A73:E75" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14">
+  <autoFilter ref="A73:E75" xr:uid="{DD8FE11C-2438-4049-A42D-CF49EF196CF3}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AE800C69-D48C-469F-8B27-8E3C20A4F9AC}" name="Testfälle" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{9B482628-9EFB-4FD6-9E7B-ACAB0F890ECC}" name="Test-Typ" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{50FD7F2C-BBD2-420D-B73E-E72326DDF9FA}" name="Bedingung" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{392B5D38-16ED-4E4B-BDE5-1FF9300EB5B0}" name="Eingaben" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{4E5CE639-7AD1-4909-B873-3887D56BA50A}" name="Erwartete Ausgaben" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F9402861-339B-44E1-87F1-41C7C73C9105}" name="Table91112" displayName="Table91112" ref="A87:E89" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="A87:E89" xr:uid="{F9402861-339B-44E1-87F1-41C7C73C9105}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{380F019D-384D-46EE-9D4E-8A5D7D3E02F9}" name="Testfälle" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{7E707297-4CC1-4F85-BC71-D446F7EAF1B6}" name="Test-Typ" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{92B23F04-44F3-4FA9-B19F-1854BE662D9F}" name="Bedingung" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8A152B66-A5CC-412B-B978-1062CFF0903C}" name="Eingaben" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{64DE1CB4-0951-457F-8A80-786DAB0086EE}" name="Erwartete Ausgaben" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F14D9A62-EDFE-495A-B364-78C15A561E64}" name="Table2" displayName="Table2" ref="A33:E37" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F14D9A62-EDFE-495A-B364-78C15A561E64}" name="Table2" displayName="Table2" ref="A33:E37" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <autoFilter ref="A33:E37" xr:uid="{F14D9A62-EDFE-495A-B364-78C15A561E64}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1FEBC6A1-198F-4391-B3DC-05D7A4E32C70}" name="Testfälle" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{042EC9E0-A8C8-4C3E-BD3F-95FC60909884}" name="Test-Typ" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{CD206702-28C3-4543-B9AF-58A1AAF95370}" name="Bedingung" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{04980909-F3A9-4833-BE87-4BB3581CB32F}" name="Eingaben" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{A6A811CF-3C68-4D81-97CA-4B50FDE26983}" name="Erwartete Ausgaben" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{1FEBC6A1-198F-4391-B3DC-05D7A4E32C70}" name="Testfälle" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{042EC9E0-A8C8-4C3E-BD3F-95FC60909884}" name="Test-Typ" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{CD206702-28C3-4543-B9AF-58A1AAF95370}" name="Bedingung" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{04980909-F3A9-4833-BE87-4BB3581CB32F}" name="Eingaben" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{A6A811CF-3C68-4D81-97CA-4B50FDE26983}" name="Erwartete Ausgaben" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BB20C13-15B3-4E38-96C9-1521AA4A3DCC}" name="Table3" displayName="Table3" ref="A12:E20" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BB20C13-15B3-4E38-96C9-1521AA4A3DCC}" name="Table3" displayName="Table3" ref="A12:E20" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A12:E20" xr:uid="{5BB20C13-15B3-4E38-96C9-1521AA4A3DCC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D5E0E3C5-5383-4429-B50C-B3998B93A4B3}" name="Testfälle" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{B697326C-9165-4043-8303-DDBF950D32F7}" name="Test-Typ" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{7FEAB877-C24A-49C7-A31C-A2708EAA40AF}" name="Bedingung" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{35F2A014-35FC-4F45-9FA0-F3FDF581AE48}" name="Eingaben" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{0931E050-95FA-4C0E-B68A-8C07BFF87033}" name="Erwartete Ausgaben" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{D5E0E3C5-5383-4429-B50C-B3998B93A4B3}" name="Testfälle" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{B697326C-9165-4043-8303-DDBF950D32F7}" name="Test-Typ" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{7FEAB877-C24A-49C7-A31C-A2708EAA40AF}" name="Bedingung" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{35F2A014-35FC-4F45-9FA0-F3FDF581AE48}" name="Eingaben" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{0931E050-95FA-4C0E-B68A-8C07BFF87033}" name="Erwartete Ausgaben" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD55EE71-C092-4977-AC10-EABA0578F3D7}" name="Table25" displayName="Table25" ref="A50:E53" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD55EE71-C092-4977-AC10-EABA0578F3D7}" name="Table25" displayName="Table25" ref="A50:E53" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
   <autoFilter ref="A50:E53" xr:uid="{BD55EE71-C092-4977-AC10-EABA0578F3D7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6D56E884-0C93-4FE3-B701-B681A7407FB0}" name="Testfälle" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6F81EE2D-6BC2-45B5-B0BC-5E496F03639C}" name="Test-Typ" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{DE80C218-9751-4F79-B688-DCC586338CAB}" name="Bedingung" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{8DA08EF7-F359-4B88-AB6B-D88B17FC13AB}" name="Eingaben" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{AEDF790C-55EA-4F5C-BBFF-833A8F1C9F11}" name="Erwartete Ausgaben" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{6D56E884-0C93-4FE3-B701-B681A7407FB0}" name="Testfälle" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{6F81EE2D-6BC2-45B5-B0BC-5E496F03639C}" name="Test-Typ" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{DE80C218-9751-4F79-B688-DCC586338CAB}" name="Bedingung" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{8DA08EF7-F359-4B88-AB6B-D88B17FC13AB}" name="Eingaben" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{AEDF790C-55EA-4F5C-BBFF-833A8F1C9F11}" name="Erwartete Ausgaben" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8CB4B03A-8958-42D0-A09E-E22577AB3C1A}" name="Table256" displayName="Table256" ref="A66:E69" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8CB4B03A-8958-42D0-A09E-E22577AB3C1A}" name="Table256" displayName="Table256" ref="A66:E69" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A66:E69" xr:uid="{8CB4B03A-8958-42D0-A09E-E22577AB3C1A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2B07C3BB-A044-42E0-8B0A-3ED55ED611E7}" name="Testfälle" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8A5EB616-F59B-4E4B-AAE2-71A879AC3B04}" name="Test-Typ" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{447637BA-270D-472C-86C4-86C5D13115E4}" name="Bedingung" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6A685376-CF34-42EA-A432-2B3B583C4522}" name="Eingaben" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{11821F10-C243-41EE-A7F8-78CF1B0BF131}" name="Erwartete Ausgaben" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{2B07C3BB-A044-42E0-8B0A-3ED55ED611E7}" name="Testfälle" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{8A5EB616-F59B-4E4B-AAE2-71A879AC3B04}" name="Test-Typ" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{447637BA-270D-472C-86C4-86C5D13115E4}" name="Bedingung" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{6A685376-CF34-42EA-A432-2B3B583C4522}" name="Eingaben" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{11821F10-C243-41EE-A7F8-78CF1B0BF131}" name="Erwartete Ausgaben" dataDxfId="50"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AED57674-1357-4261-869F-C4F770D1964C}" name="Table6" displayName="Table6" ref="A11:E15" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="49">
+  <autoFilter ref="A11:E15" xr:uid="{AED57674-1357-4261-869F-C4F770D1964C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D45BAFD3-A17D-431E-A8DC-0E586886C6BB}" name="Testfälle" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{A3CE828B-7A65-467A-A484-062F81D7BDD1}" name="Test-Typ" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{028F41C1-7F89-4C55-993D-3E7BA8DA2F4A}" name="Bedingung" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{3B4326D2-7A2B-4E7A-81C0-0855A0DFAD77}" name="Eingaben" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{DA7E9238-5A08-41F6-9B37-0978E74DA15A}" name="Erwartete Ausgaben" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2AA13F25-C7B4-4238-AA3B-A23A8A0253F2}" name="Table7" displayName="Table7" ref="A27:E29" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="45" tableBorderDxfId="46" totalsRowBorderDxfId="44">
+  <autoFilter ref="A27:E29" xr:uid="{2AA13F25-C7B4-4238-AA3B-A23A8A0253F2}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E0138A14-BE39-41AE-866E-DB95741FBD27}" name="Testfälle" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{81328A7E-884D-48AC-AE97-26945A402043}" name="Test-Typ" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{72D69D40-E618-48A4-8232-F80581710D31}" name="Bedingung" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{B5E56898-1B46-4544-B438-34BC21E421EF}" name="Eingaben" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{1E2F340E-5A77-4A0B-A68F-1C771FE3AB61}" name="Erwartete Ausgaben" dataDxfId="26"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9F5396AA-74C9-440E-9500-082F97418ED5}" name="Table8" displayName="Table8" ref="A41:E45" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="36" tableBorderDxfId="37" totalsRowBorderDxfId="35">
+  <autoFilter ref="A41:E45" xr:uid="{9F5396AA-74C9-440E-9500-082F97418ED5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6FE4AB55-E2B7-435E-B8B6-1591B0B4151E}" name="Testfälle" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{58B37ADE-0E63-4838-8060-71C2CFEC70CE}" name="Test-Typ" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{FA04D83D-CF54-47E0-921B-E80B3D048729}" name="Bedingung" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{CCC6ECED-0112-48EE-A977-ED97707A7256}" name="Eingaben" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{8133A33E-4E37-4E57-8A60-8DC84EFCD208}" name="Erwartete Ausgaben" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F58F2C59-255E-4965-A03B-94F0CEA13384}" name="Table9" displayName="Table9" ref="A57:E61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="33">
+  <autoFilter ref="A57:E61" xr:uid="{F58F2C59-255E-4965-A03B-94F0CEA13384}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0BA2FEF2-3570-4836-B9EA-2A9F7AA09852}" name="Testfälle" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{5BC540B2-644D-4AB1-A610-65BED07CB54A}" name="Test-Typ" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F1B0A6F4-1E7A-408F-80CB-212672B7B8C9}" name="Bedingung" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{7DC05564-FF9E-40A3-B5E2-D05D8CC344B1}" name="Eingaben" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{2219C4F7-38D9-4E60-B28B-470ADEFB72FF}" name="Erwartete Ausgaben" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1803,7 +2991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA8CA56-581F-4991-9983-10E0961810A1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1838,7 +3026,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>44</v>
@@ -1847,7 +3035,7 @@
         <v>45</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1866,8 +3054,8 @@
       <c r="E5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>142</v>
+      <c r="F5" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1886,8 +3074,8 @@
       <c r="E6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>142</v>
+      <c r="F6" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1906,8 +3094,8 @@
       <c r="E7" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>142</v>
+      <c r="F7" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,8 +3114,8 @@
       <c r="E8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>142</v>
+      <c r="F8" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2018,8 +3206,8 @@
       <c r="E13" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>143</v>
+      <c r="F13" s="30" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2038,8 +3226,8 @@
       <c r="E14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>144</v>
+      <c r="F14" s="30" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2047,19 +3235,19 @@
         <v>40</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2074,7 +3262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5777E552-38DB-4FF6-8E00-150ECCF800EA}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2358,8 +3548,8 @@
       <c r="D20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>100</v>
+      <c r="E20" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2777,7 +3967,7 @@
         <v>91</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D62" s="2"/>
     </row>
@@ -2798,13 +3988,13 @@
         <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2838,7 +4028,7 @@
         <v>94</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,7 +4045,7 @@
         <v>94</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2866,13 +4056,13 @@
         <v>79</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3237,297 +4427,297 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="31">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="32">
+        <v>2</v>
+      </c>
+      <c r="B21" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="31">
-        <v>2</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3544,12 +4734,967 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC10DF8B-338F-4ED2-9F64-130340EF975F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="12">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="12">
+        <v>3</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="12">
+        <v>1</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="12">
+        <v>2</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="12">
+        <v>3</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="12">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="24"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="12">
+        <v>1</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="12">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="24"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" s="21"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="12">
+        <v>1</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="12">
+        <v>2</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="6">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>